<commit_message>
Cambio de forma de cálculo de tasaciones y Matriz según indicaciones de Gerencia TAS
</commit_message>
<xml_diff>
--- a/pytasks/Formatos/Vr 0/MATRIZ TASACIONES- REv.xlsx
+++ b/pytasks/Formatos/Vr 0/MATRIZ TASACIONES- REv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pollo\OneDrive\Development\1- Bienes Futuros\tasks\Formatos\Vr 0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pollo\OneDrive\Development\1-BienesFuturos\pytasks\Formatos\Vr 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE8E946-22AA-44AC-BE90-9CB3CD27855F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F4CB03-730E-4684-ADAA-2DA45B3B36E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="2010" windowWidth="21600" windowHeight="11505" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRIZ" sheetId="3" r:id="rId1"/>
@@ -886,22 +886,10 @@
     <xf numFmtId="41" fontId="1" fillId="2" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -926,6 +914,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2603,12 +2603,12 @@
   </sheetPr>
   <dimension ref="A1:AG247"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="11" topLeftCell="D225" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <pane xSplit="3" ySplit="11" topLeftCell="P12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AA81" sqref="AA81"/>
       <selection pane="topRight" activeCell="AA81" sqref="AA81"/>
       <selection pane="bottomLeft" activeCell="AA81" sqref="AA81"/>
-      <selection pane="bottomRight" activeCell="F236" sqref="F236"/>
+      <selection pane="bottomRight" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2686,8 +2686,8 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
       <c r="F3" s="10"/>
       <c r="G3" s="49"/>
       <c r="H3" s="1" t="s">
@@ -2703,8 +2703,8 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="10"/>
       <c r="G4" s="50"/>
       <c r="H4" s="1" t="s">
@@ -2721,8 +2721,8 @@
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="10"/>
       <c r="G5" s="64" t="s">
         <v>46</v>
@@ -2737,8 +2737,8 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
       <c r="F6" s="10"/>
       <c r="G6" s="65" t="s">
         <v>88</v>
@@ -2754,11 +2754,11 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="74">
+      <c r="D7" s="84">
         <f>+MAX(Tabla2[Fecha de Tasación])</f>
         <v>0</v>
       </c>
-      <c r="E7" s="74"/>
+      <c r="E7" s="84"/>
       <c r="F7" s="10"/>
       <c r="L7" s="12"/>
       <c r="AD7" s="2"/>
@@ -2770,8 +2770,8 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
       <c r="F8" s="8" t="s">
         <v>18</v>
       </c>
@@ -2798,32 +2798,32 @@
       <c r="B10" s="3"/>
       <c r="D10" s="13"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="80" t="s">
+      <c r="F10" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="77" t="s">
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="78"/>
-      <c r="T10" s="78"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="78"/>
-      <c r="W10" s="78"/>
-      <c r="X10" s="78"/>
-      <c r="Y10" s="78"/>
-      <c r="Z10" s="78"/>
-      <c r="AA10" s="79"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="75"/>
       <c r="AB10" s="2"/>
       <c r="AF10" s="42"/>
     </row>
@@ -29300,176 +29300,176 @@
         <v>19</v>
       </c>
       <c r="C240" s="25"/>
-      <c r="D240" s="83" t="s">
+      <c r="D240" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="E240" s="84"/>
+      <c r="E240" s="80"/>
       <c r="G240" s="21"/>
       <c r="AB240" s="16"/>
     </row>
     <row r="241" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C241" s="26"/>
-      <c r="D241" s="72" t="s">
+      <c r="D241" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E241" s="73"/>
+      <c r="E241" s="83"/>
       <c r="AB241" s="16"/>
     </row>
     <row r="242" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AB242" s="16"/>
     </row>
     <row r="243" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="75" t="s">
+      <c r="A243" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B243" s="75"/>
-      <c r="C243" s="70" t="s">
+      <c r="B243" s="70"/>
+      <c r="C243" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="D243" s="70"/>
-      <c r="E243" s="70"/>
-      <c r="F243" s="70"/>
-      <c r="G243" s="70"/>
-      <c r="H243" s="70"/>
-      <c r="I243" s="70"/>
-      <c r="J243" s="70"/>
-      <c r="K243" s="70"/>
-      <c r="L243" s="70"/>
-      <c r="M243" s="70"/>
-      <c r="N243" s="70"/>
-      <c r="O243" s="70"/>
-      <c r="P243" s="70"/>
-      <c r="Q243" s="70"/>
-      <c r="R243" s="70"/>
-      <c r="S243" s="70"/>
-      <c r="T243" s="70"/>
-      <c r="U243" s="70"/>
-      <c r="V243" s="70"/>
-      <c r="W243" s="70"/>
-      <c r="X243" s="70"/>
-      <c r="Y243" s="70"/>
-      <c r="Z243" s="70"/>
-      <c r="AA243" s="70"/>
+      <c r="D243" s="71"/>
+      <c r="E243" s="71"/>
+      <c r="F243" s="71"/>
+      <c r="G243" s="71"/>
+      <c r="H243" s="71"/>
+      <c r="I243" s="71"/>
+      <c r="J243" s="71"/>
+      <c r="K243" s="71"/>
+      <c r="L243" s="71"/>
+      <c r="M243" s="71"/>
+      <c r="N243" s="71"/>
+      <c r="O243" s="71"/>
+      <c r="P243" s="71"/>
+      <c r="Q243" s="71"/>
+      <c r="R243" s="71"/>
+      <c r="S243" s="71"/>
+      <c r="T243" s="71"/>
+      <c r="U243" s="71"/>
+      <c r="V243" s="71"/>
+      <c r="W243" s="71"/>
+      <c r="X243" s="71"/>
+      <c r="Y243" s="71"/>
+      <c r="Z243" s="71"/>
+      <c r="AA243" s="71"/>
       <c r="AB243" s="16"/>
     </row>
     <row r="244" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C244" s="70" t="s">
+      <c r="C244" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D244" s="70"/>
-      <c r="E244" s="70"/>
-      <c r="F244" s="70"/>
-      <c r="G244" s="70"/>
-      <c r="H244" s="70"/>
-      <c r="I244" s="70"/>
-      <c r="J244" s="70"/>
-      <c r="K244" s="70"/>
-      <c r="L244" s="70"/>
-      <c r="M244" s="70"/>
-      <c r="N244" s="70"/>
-      <c r="O244" s="70"/>
-      <c r="P244" s="70"/>
-      <c r="Q244" s="70"/>
-      <c r="R244" s="70"/>
-      <c r="S244" s="70"/>
-      <c r="T244" s="70"/>
-      <c r="U244" s="70"/>
-      <c r="V244" s="70"/>
-      <c r="W244" s="70"/>
-      <c r="X244" s="70"/>
-      <c r="Y244" s="70"/>
-      <c r="Z244" s="70"/>
-      <c r="AA244" s="70"/>
+      <c r="D244" s="71"/>
+      <c r="E244" s="71"/>
+      <c r="F244" s="71"/>
+      <c r="G244" s="71"/>
+      <c r="H244" s="71"/>
+      <c r="I244" s="71"/>
+      <c r="J244" s="71"/>
+      <c r="K244" s="71"/>
+      <c r="L244" s="71"/>
+      <c r="M244" s="71"/>
+      <c r="N244" s="71"/>
+      <c r="O244" s="71"/>
+      <c r="P244" s="71"/>
+      <c r="Q244" s="71"/>
+      <c r="R244" s="71"/>
+      <c r="S244" s="71"/>
+      <c r="T244" s="71"/>
+      <c r="U244" s="71"/>
+      <c r="V244" s="71"/>
+      <c r="W244" s="71"/>
+      <c r="X244" s="71"/>
+      <c r="Y244" s="71"/>
+      <c r="Z244" s="71"/>
+      <c r="AA244" s="71"/>
       <c r="AB244" s="16"/>
     </row>
     <row r="245" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C245" s="76" t="s">
+      <c r="C245" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="D245" s="76"/>
-      <c r="E245" s="76"/>
-      <c r="F245" s="76"/>
-      <c r="G245" s="76"/>
-      <c r="H245" s="76"/>
-      <c r="I245" s="76"/>
-      <c r="J245" s="76"/>
-      <c r="K245" s="76"/>
-      <c r="L245" s="76"/>
-      <c r="M245" s="76"/>
-      <c r="N245" s="76"/>
-      <c r="O245" s="76"/>
-      <c r="P245" s="76"/>
-      <c r="Q245" s="76"/>
-      <c r="R245" s="76"/>
-      <c r="S245" s="76"/>
-      <c r="T245" s="76"/>
-      <c r="U245" s="76"/>
-      <c r="V245" s="76"/>
-      <c r="W245" s="76"/>
-      <c r="X245" s="76"/>
-      <c r="Y245" s="76"/>
-      <c r="Z245" s="76"/>
-      <c r="AA245" s="76"/>
+      <c r="D245" s="72"/>
+      <c r="E245" s="72"/>
+      <c r="F245" s="72"/>
+      <c r="G245" s="72"/>
+      <c r="H245" s="72"/>
+      <c r="I245" s="72"/>
+      <c r="J245" s="72"/>
+      <c r="K245" s="72"/>
+      <c r="L245" s="72"/>
+      <c r="M245" s="72"/>
+      <c r="N245" s="72"/>
+      <c r="O245" s="72"/>
+      <c r="P245" s="72"/>
+      <c r="Q245" s="72"/>
+      <c r="R245" s="72"/>
+      <c r="S245" s="72"/>
+      <c r="T245" s="72"/>
+      <c r="U245" s="72"/>
+      <c r="V245" s="72"/>
+      <c r="W245" s="72"/>
+      <c r="X245" s="72"/>
+      <c r="Y245" s="72"/>
+      <c r="Z245" s="72"/>
+      <c r="AA245" s="72"/>
       <c r="AB245" s="16"/>
     </row>
     <row r="246" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C246" s="70" t="s">
+      <c r="C246" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D246" s="70"/>
-      <c r="E246" s="70"/>
-      <c r="F246" s="70"/>
-      <c r="G246" s="70"/>
-      <c r="H246" s="70"/>
-      <c r="I246" s="70"/>
-      <c r="J246" s="70"/>
-      <c r="K246" s="70"/>
-      <c r="L246" s="70"/>
-      <c r="M246" s="70"/>
-      <c r="N246" s="70"/>
-      <c r="O246" s="70"/>
-      <c r="P246" s="70"/>
-      <c r="Q246" s="70"/>
-      <c r="R246" s="70"/>
-      <c r="S246" s="70"/>
-      <c r="T246" s="70"/>
-      <c r="U246" s="70"/>
-      <c r="V246" s="70"/>
-      <c r="W246" s="70"/>
-      <c r="X246" s="70"/>
-      <c r="Y246" s="70"/>
-      <c r="Z246" s="70"/>
-      <c r="AA246" s="70"/>
+      <c r="D246" s="71"/>
+      <c r="E246" s="71"/>
+      <c r="F246" s="71"/>
+      <c r="G246" s="71"/>
+      <c r="H246" s="71"/>
+      <c r="I246" s="71"/>
+      <c r="J246" s="71"/>
+      <c r="K246" s="71"/>
+      <c r="L246" s="71"/>
+      <c r="M246" s="71"/>
+      <c r="N246" s="71"/>
+      <c r="O246" s="71"/>
+      <c r="P246" s="71"/>
+      <c r="Q246" s="71"/>
+      <c r="R246" s="71"/>
+      <c r="S246" s="71"/>
+      <c r="T246" s="71"/>
+      <c r="U246" s="71"/>
+      <c r="V246" s="71"/>
+      <c r="W246" s="71"/>
+      <c r="X246" s="71"/>
+      <c r="Y246" s="71"/>
+      <c r="Z246" s="71"/>
+      <c r="AA246" s="71"/>
       <c r="AB246" s="16"/>
     </row>
     <row r="247" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C247" s="70" t="s">
+      <c r="C247" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D247" s="70"/>
-      <c r="E247" s="70"/>
-      <c r="F247" s="70"/>
-      <c r="G247" s="70"/>
-      <c r="H247" s="70"/>
-      <c r="I247" s="70"/>
-      <c r="J247" s="70"/>
-      <c r="K247" s="70"/>
-      <c r="L247" s="70"/>
-      <c r="M247" s="70"/>
-      <c r="N247" s="70"/>
-      <c r="O247" s="70"/>
-      <c r="P247" s="70"/>
-      <c r="Q247" s="70"/>
-      <c r="R247" s="70"/>
-      <c r="S247" s="70"/>
-      <c r="T247" s="70"/>
-      <c r="U247" s="70"/>
-      <c r="V247" s="70"/>
-      <c r="W247" s="70"/>
-      <c r="X247" s="70"/>
-      <c r="Y247" s="70"/>
-      <c r="Z247" s="70"/>
-      <c r="AA247" s="70"/>
+      <c r="D247" s="71"/>
+      <c r="E247" s="71"/>
+      <c r="F247" s="71"/>
+      <c r="G247" s="71"/>
+      <c r="H247" s="71"/>
+      <c r="I247" s="71"/>
+      <c r="J247" s="71"/>
+      <c r="K247" s="71"/>
+      <c r="L247" s="71"/>
+      <c r="M247" s="71"/>
+      <c r="N247" s="71"/>
+      <c r="O247" s="71"/>
+      <c r="P247" s="71"/>
+      <c r="Q247" s="71"/>
+      <c r="R247" s="71"/>
+      <c r="S247" s="71"/>
+      <c r="T247" s="71"/>
+      <c r="U247" s="71"/>
+      <c r="V247" s="71"/>
+      <c r="W247" s="71"/>
+      <c r="X247" s="71"/>
+      <c r="Y247" s="71"/>
+      <c r="Z247" s="71"/>
+      <c r="AA247" s="71"/>
       <c r="AB247" s="16"/>
     </row>
   </sheetData>
@@ -29479,13 +29479,6 @@
     <sortCondition ref="D239:D268"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="A243:B243"/>
-    <mergeCell ref="C243:AA243"/>
-    <mergeCell ref="C244:AA244"/>
-    <mergeCell ref="C245:AA245"/>
-    <mergeCell ref="L10:AA10"/>
-    <mergeCell ref="F10:K10"/>
-    <mergeCell ref="D240:E240"/>
     <mergeCell ref="C246:AA246"/>
     <mergeCell ref="C247:AA247"/>
     <mergeCell ref="D3:E3"/>
@@ -29495,6 +29488,13 @@
     <mergeCell ref="D241:E241"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A243:B243"/>
+    <mergeCell ref="C243:AA243"/>
+    <mergeCell ref="C244:AA244"/>
+    <mergeCell ref="C245:AA245"/>
+    <mergeCell ref="L10:AA10"/>
+    <mergeCell ref="F10:K10"/>
+    <mergeCell ref="D240:E240"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:I12 K12:AG12">
     <cfRule type="expression" dxfId="47" priority="13">
@@ -29556,7 +29556,7 @@
       <formula>$AA13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD12:AD237" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Vista</formula1>
     </dataValidation>

</xml_diff>